<commit_message>
fix tests and test data
</commit_message>
<xml_diff>
--- a/testdata/invalid-testdata/excel2json/properties-invalid-gui_attribute.xlsx
+++ b/testdata/invalid-testdata/excel2json/properties-invalid-gui_attribute.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -94,25 +94,28 @@
     <t>Geonames</t>
   </si>
   <si>
-    <t>hasInterval</t>
-  </si>
-  <si>
-    <t>Time interval</t>
-  </si>
-  <si>
-    <t>Zeitintervall</t>
-  </si>
-  <si>
-    <t>hasSequenceBounds</t>
-  </si>
-  <si>
-    <t>IntervalValue</t>
-  </si>
-  <si>
-    <t>SimpleText</t>
-  </si>
-  <si>
-    <t>maxlength: 5, rows: 10</t>
+    <t>hasInteger</t>
+  </si>
+  <si>
+    <t>has Integer</t>
+  </si>
+  <si>
+    <t>Zahl</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>zahl</t>
+  </si>
+  <si>
+    <t>IntValue</t>
+  </si>
+  <si>
+    <t>Spinbox</t>
+  </si>
+  <si>
+    <t>max: 10, min: 5, rows: 10</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -673,31 +676,31 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
       <c r="L4" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -707,7 +710,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>

</xml_diff>

<commit_message>
chore: replace gui_element Slider by Spinbox, remove gui_element SimpleText for intervals, et al. (DEV-2501) (#452)
</commit_message>
<xml_diff>
--- a/testdata/invalid-testdata/excel2json/properties-invalid-gui_attribute.xlsx
+++ b/testdata/invalid-testdata/excel2json/properties-invalid-gui_attribute.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -94,25 +94,28 @@
     <t>Geonames</t>
   </si>
   <si>
-    <t>hasInterval</t>
-  </si>
-  <si>
-    <t>Time interval</t>
-  </si>
-  <si>
-    <t>Zeitintervall</t>
-  </si>
-  <si>
-    <t>hasSequenceBounds</t>
-  </si>
-  <si>
-    <t>IntervalValue</t>
-  </si>
-  <si>
-    <t>SimpleText</t>
-  </si>
-  <si>
-    <t>maxlength: 5, rows: 10</t>
+    <t>hasInteger</t>
+  </si>
+  <si>
+    <t>has Integer</t>
+  </si>
+  <si>
+    <t>Zahl</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>zahl</t>
+  </si>
+  <si>
+    <t>IntValue</t>
+  </si>
+  <si>
+    <t>Spinbox</t>
+  </si>
+  <si>
+    <t>max: 10, min: 5, rows: 10</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -673,31 +676,31 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
       <c r="L4" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -707,7 +710,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>

</xml_diff>